<commit_message>
adding code for fundManager, including units/assetCat into grouped data
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3790043-D6F3-4160-9995-B7256E45DF58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F6632-A16F-4289-BEA9-C7EC9758F1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="12961" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="12961" activeTab="1" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fund_details" sheetId="1" r:id="rId1"/>
+    <sheet name="fund_map" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>T. Rowe Price</t>
   </si>
@@ -88,6 +89,195 @@
   </si>
   <si>
     <t>http://www.wellington.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BARONFUNDS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BlackRock-Advised Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BlackRock-advised Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'CRMCFNDGRP'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Davis Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Delaware Funds by Macquarie'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FIRSTPACAD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Federated Hermes Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Fidelity Group of Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Franklin Templeton Group of Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Goldman Sachs Fund Complex'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Guggenheim'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'HARTFORD FUNDS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'INVESCOFDS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'JNL Fund Complex'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'John Hancock Group of Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LINCOLNTRS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MASSMUTUAL FUNDS'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Neuberger Berman'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Principal Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Publicly registered funds managed by Blackstone Alternative Asset Management L.P. Blackstone Alternative Investment Advisors LLC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SUNAMERICA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Selected Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TROWEPRICE'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'VALIC Company'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Voya mutual funds'</t>
+  </si>
+  <si>
+    <t>'Azzad Funds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Brighthouse Funds Trust I'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Brighthouse Funds Trust II'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Brinker Capital Destinations Trust'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Clipper Funds Trust'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'GREAT-WEST FUNDS INC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PENN SERIES FUNDS INC'</t>
+  </si>
+  <si>
+    <t>fundManager_raw</t>
+  </si>
+  <si>
+    <t>fundManager</t>
+  </si>
+  <si>
+    <t>Azzad</t>
+  </si>
+  <si>
+    <t>BlackRock</t>
+  </si>
+  <si>
+    <t>Brighthouse</t>
+  </si>
+  <si>
+    <t>Clipper</t>
+  </si>
+  <si>
+    <t>Baron</t>
+  </si>
+  <si>
+    <t>Brinker Capital</t>
+  </si>
+  <si>
+    <t>Federated Hermes</t>
+  </si>
+  <si>
+    <t>Franklin Templeton</t>
+  </si>
+  <si>
+    <t>Goldman Sachs</t>
+  </si>
+  <si>
+    <t>John Hancock</t>
+  </si>
+  <si>
+    <t>Guggenheim</t>
+  </si>
+  <si>
+    <t>Neuberger Berman</t>
+  </si>
+  <si>
+    <t>Principal Funds</t>
+  </si>
+  <si>
+    <t>Selected Funds</t>
+  </si>
+  <si>
+    <t>Invesco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davis </t>
+  </si>
+  <si>
+    <t>Macquarie</t>
+  </si>
+  <si>
+    <t>Great-West</t>
+  </si>
+  <si>
+    <t>Voya</t>
+  </si>
+  <si>
+    <t>Sun America</t>
+  </si>
+  <si>
+    <t>Jackson National</t>
+  </si>
+  <si>
+    <t>Lincoln Investment</t>
+  </si>
+  <si>
+    <t>MassMutual</t>
+  </si>
+  <si>
+    <t>PennMutual</t>
+  </si>
+  <si>
+    <t>VALIC</t>
+  </si>
+  <si>
+    <t>Blackstone</t>
+  </si>
+  <si>
+    <t>First Pacific Advisors</t>
+  </si>
+  <si>
+    <t>Capital Group</t>
   </si>
 </sst>
 </file>
@@ -452,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728DFE42-5040-4D37-A18F-76721B3D167B}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,4 +728,295 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54B6945-86F8-4783-8FF1-FE1348B6CFC5}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed back to fundManager with manually adjusted names. fixed sec html links
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F6632-A16F-4289-BEA9-C7EC9758F1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4795018-692B-4EC0-83FD-8D0879B73624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="12961" activeTab="1" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
   <sheets>
     <sheet name="fund_details" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>T. Rowe Price</t>
   </si>
@@ -91,105 +91,6 @@
     <t>http://www.wellington.com</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'BARONFUNDS'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'BlackRock-Advised Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'BlackRock-advised Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'CRMCFNDGRP'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Davis Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Delaware Funds by Macquarie'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'FIRSTPACAD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Federated Hermes Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Fidelity Group of Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Franklin Templeton Group of Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Goldman Sachs Fund Complex'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Guggenheim'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'HARTFORD FUNDS'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'INVESCOFDS'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'JNL Fund Complex'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'John Hancock Group of Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'LINCOLNTRS'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'MASSMUTUAL FUNDS'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Neuberger Berman'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Principal Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Publicly registered funds managed by Blackstone Alternative Asset Management L.P. Blackstone Alternative Investment Advisors LLC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'SUNAMERICA'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Selected Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'TROWEPRICE'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'VALIC Company'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Voya mutual funds'</t>
-  </si>
-  <si>
-    <t>'Azzad Funds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Brighthouse Funds Trust I'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Brighthouse Funds Trust II'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Brinker Capital Destinations Trust'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Clipper Funds Trust'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'GREAT-WEST FUNDS INC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'PENN SERIES FUNDS INC'</t>
-  </si>
-  <si>
     <t>fundManager_raw</t>
   </si>
   <si>
@@ -214,6 +115,9 @@
     <t>Brinker Capital</t>
   </si>
   <si>
+    <t>Delaware Funds</t>
+  </si>
+  <si>
     <t>Federated Hermes</t>
   </si>
   <si>
@@ -226,27 +130,90 @@
     <t>John Hancock</t>
   </si>
   <si>
+    <t>Azzad Funds</t>
+  </si>
+  <si>
+    <t>CRMCFNDGRP</t>
+  </si>
+  <si>
+    <t>Davis Funds</t>
+  </si>
+  <si>
+    <t>Delaware Funds by Macquarie</t>
+  </si>
+  <si>
+    <t>FIRSTPACAD</t>
+  </si>
+  <si>
+    <t>Federated Hermes Funds</t>
+  </si>
+  <si>
+    <t>Fidelity Group of Funds</t>
+  </si>
+  <si>
+    <t>Franklin Templeton Group of Funds</t>
+  </si>
+  <si>
+    <t>GREAT-WEST FUNDS INC</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Fund Complex</t>
+  </si>
+  <si>
     <t>Guggenheim</t>
   </si>
   <si>
+    <t>HARTFORD FUNDS</t>
+  </si>
+  <si>
+    <t>INVESCOFDS</t>
+  </si>
+  <si>
+    <t>JNL Fund Complex</t>
+  </si>
+  <si>
+    <t>John Hancock Group of Funds</t>
+  </si>
+  <si>
+    <t>LINCOLNTRS</t>
+  </si>
+  <si>
+    <t>MASSMUTUAL FUNDS</t>
+  </si>
+  <si>
     <t>Neuberger Berman</t>
   </si>
   <si>
+    <t>PENN SERIES FUNDS INC</t>
+  </si>
+  <si>
     <t>Principal Funds</t>
   </si>
   <si>
+    <t>Publicly registered funds managed by Blackstone Alternative Asset Management L.P. Blackstone Alternative Investment Advisors LLC</t>
+  </si>
+  <si>
+    <t>SUNAMERICA</t>
+  </si>
+  <si>
     <t>Selected Funds</t>
   </si>
   <si>
+    <t>TROWEPRICE</t>
+  </si>
+  <si>
+    <t>VALIC Company</t>
+  </si>
+  <si>
+    <t>Voya mutual funds</t>
+  </si>
+  <si>
     <t>Invesco</t>
   </si>
   <si>
     <t xml:space="preserve">Davis </t>
   </si>
   <si>
-    <t>Macquarie</t>
-  </si>
-  <si>
     <t>Great-West</t>
   </si>
   <si>
@@ -265,9 +232,6 @@
     <t>MassMutual</t>
   </si>
   <si>
-    <t>PennMutual</t>
-  </si>
-  <si>
     <t>VALIC</t>
   </si>
   <si>
@@ -278,6 +242,30 @@
   </si>
   <si>
     <t>Capital Group</t>
+  </si>
+  <si>
+    <t>BARONFUNDS</t>
+  </si>
+  <si>
+    <t>BlackRock-Advised Funds</t>
+  </si>
+  <si>
+    <t>BlackRock-advised Funds</t>
+  </si>
+  <si>
+    <t>Brighthouse Funds Trust I</t>
+  </si>
+  <si>
+    <t>Brighthouse Funds Trust II</t>
+  </si>
+  <si>
+    <t>Brinker Capital Destinations Trust</t>
+  </si>
+  <si>
+    <t>Clipper Funds Trust</t>
+  </si>
+  <si>
+    <t>Penn Mutual</t>
   </si>
 </sst>
 </file>
@@ -735,7 +723,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,119 +734,119 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -866,39 +854,39 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -906,55 +894,55 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
@@ -962,39 +950,39 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1002,18 +990,18 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fund logos, font in datatables
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4795018-692B-4EC0-83FD-8D0879B73624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB3BB3-94CE-4B75-992C-5F932F632A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
   <sheets>
     <sheet name="fund_details" sheetId="1" r:id="rId1"/>
@@ -35,20 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>T. Rowe Price</t>
   </si>
   <si>
-    <t>Blackrock</t>
-  </si>
-  <si>
     <t>Fidelity</t>
   </si>
   <si>
-    <t>Wellington Management</t>
-  </si>
-  <si>
     <t>Hartford Funds</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>t_rowe_price-logo.png</t>
   </si>
   <si>
-    <t>wellington-logo.png</t>
-  </si>
-  <si>
     <t>http://www.blackrock.com</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>http://www.troweprice.com</t>
   </si>
   <si>
-    <t>http://www.wellington.com</t>
-  </si>
-  <si>
     <t>fundManager_raw</t>
   </si>
   <si>
@@ -266,6 +254,42 @@
   </si>
   <si>
     <t>Penn Mutual</t>
+  </si>
+  <si>
+    <t>capital_group-logo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.capitalgroup.com</t>
+  </si>
+  <si>
+    <t>davis-logo.gif</t>
+  </si>
+  <si>
+    <t>https://www.davisadvisors.com</t>
+  </si>
+  <si>
+    <t>franklin_templeton-logo.png</t>
+  </si>
+  <si>
+    <t>https://www.franklintempleton.com</t>
+  </si>
+  <si>
+    <t>https://www.invesco.com</t>
+  </si>
+  <si>
+    <t>invesco-logo.jpg</t>
+  </si>
+  <si>
+    <t>massmutual-logo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.massmutual.com/mmfunds</t>
+  </si>
+  <si>
+    <t>principal-logo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.principalfunds.com</t>
   </si>
 </sst>
 </file>
@@ -628,91 +652,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728DFE42-5040-4D37-A18F-76721B3D167B}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{DE9206EF-784B-404E-AA4D-FC109CC8C962}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{664837A7-9452-43BD-8E05-D2931F1E689B}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{B9EAD88A-DF2F-4FB7-8CFF-31BD06CC9AAD}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{84F737F8-D8B7-4FC7-BB40-05896703648A}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{EB1D0608-3E8D-4D23-A59C-4D040B193CB6}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{664837A7-9452-43BD-8E05-D2931F1E689B}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{84F737F8-D8B7-4FC7-BB40-05896703648A}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{EB1D0608-3E8D-4D23-A59C-4D040B193CB6}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{B8D59B1E-1160-4845-B990-CBA9E689B0B0}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{63C00469-1F70-4635-95AE-5D6FCA08E692}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{08B9DFBE-B236-4903-83E7-D976326E4A6F}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{B5AD4173-60F9-448D-B6B1-DEE863EF893C}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{69314D2E-6DC3-425F-9EA7-CBDE1E0771BB}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{6D27A40A-E4F2-4E60-AB06-DBA72D94B37E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -722,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54B6945-86F8-4783-8FF1-FE1348B6CFC5}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,255 +821,255 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -990,18 +1077,18 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
         <v>56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created map_fundManager() in load_ciks, changed app_summary from fundfamily to fundManager, mapped fundManager for allfunds, no update in app_search if key word returns no results
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB3BB3-94CE-4B75-992C-5F932F632A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC8FDBB-486E-4772-9B0C-CBF516FC5F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="2" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
   <sheets>
     <sheet name="fund_details" sheetId="1" r:id="rId1"/>
     <sheet name="fund_map" sheetId="2" r:id="rId2"/>
+    <sheet name="allfund_map" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">allfund_map!$A$1:$B$156</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="305">
   <si>
     <t>T. Rowe Price</t>
   </si>
@@ -184,6 +188,9 @@
     <t>SUNAMERICA</t>
   </si>
   <si>
+    <t>Frank Funds</t>
+  </si>
+  <si>
     <t>Selected Funds</t>
   </si>
   <si>
@@ -290,6 +297,663 @@
   </si>
   <si>
     <t>https://www.principalfunds.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALLIANZ FUNDS</t>
+  </si>
+  <si>
+    <t>ABERDEENFU</t>
+  </si>
+  <si>
+    <t>AIG Mutual Funds</t>
+  </si>
+  <si>
+    <t>ALGER FUNDS</t>
+  </si>
+  <si>
+    <t>ALGERFUNDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALGERFUNDS </t>
+  </si>
+  <si>
+    <t>ALLIANCEBE</t>
+  </si>
+  <si>
+    <t>ALPS Advised Funds</t>
+  </si>
+  <si>
+    <t>AMGFUNDSGR</t>
+  </si>
+  <si>
+    <t>AQR Funds</t>
+  </si>
+  <si>
+    <t>Allianz Global</t>
+  </si>
+  <si>
+    <t>Alpha Architect ETF Trust</t>
+  </si>
+  <si>
+    <t>AmericaFirst Quantitative Funds</t>
+  </si>
+  <si>
+    <t>American Beacon</t>
+  </si>
+  <si>
+    <t>Angel Oak Funds</t>
+  </si>
+  <si>
+    <t>Ashmore Funds</t>
+  </si>
+  <si>
+    <t>BBH TRUST</t>
+  </si>
+  <si>
+    <t>BRIDGE BUILDER TRUST</t>
+  </si>
+  <si>
+    <t>COHENSTEER</t>
+  </si>
+  <si>
+    <t>COMMUNITY CAPITAL TRUST</t>
+  </si>
+  <si>
+    <t>Calvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City National Rochdale Funds               </t>
+  </si>
+  <si>
+    <t>Columbia Funds Complex</t>
+  </si>
+  <si>
+    <t>Credit Suisse</t>
+  </si>
+  <si>
+    <t>Crossmark Global Investments</t>
+  </si>
+  <si>
+    <t>DWS Funds</t>
+  </si>
+  <si>
+    <t>Direxion Shares ETF Trust</t>
+  </si>
+  <si>
+    <t>DoubleLine Funds</t>
+  </si>
+  <si>
+    <t>EATONVANCE</t>
+  </si>
+  <si>
+    <t>EQFUNDS</t>
+  </si>
+  <si>
+    <t>ETF Managers Trust</t>
+  </si>
+  <si>
+    <t>EatonVance</t>
+  </si>
+  <si>
+    <t>FRANKLIN TEMPLETON GROUP OF FUNDS</t>
+  </si>
+  <si>
+    <t>First Eagle Funds</t>
+  </si>
+  <si>
+    <t>First Trust Advisors L.P</t>
+  </si>
+  <si>
+    <t>First Trust Advisors L.P.</t>
+  </si>
+  <si>
+    <t>Franklin Templeton Group of funds</t>
+  </si>
+  <si>
+    <t>GLENMEDEFU</t>
+  </si>
+  <si>
+    <t>GMO Mutual Funds</t>
+  </si>
+  <si>
+    <t>Gabelli/GAMCO Fund Complex</t>
+  </si>
+  <si>
+    <t>Gabelli/GAMCO/Teton/Keeley Complex</t>
+  </si>
+  <si>
+    <t>Global X Funds</t>
+  </si>
+  <si>
+    <t>GuideMark and GuidePath Funds</t>
+  </si>
+  <si>
+    <t>Highland Funds</t>
+  </si>
+  <si>
+    <t>Highland Funds Complex</t>
+  </si>
+  <si>
+    <t>INVESCOETF</t>
+  </si>
+  <si>
+    <t>INVESTMENT MANAGERS SERIES TRUST</t>
+  </si>
+  <si>
+    <t>INVESTMENT MANAGERS SERIES TRUST II</t>
+  </si>
+  <si>
+    <t>IVY FUNDS</t>
+  </si>
+  <si>
+    <t>IndexIQ</t>
+  </si>
+  <si>
+    <t>Innovator ETFs Trust</t>
+  </si>
+  <si>
+    <t>Integrity Viking Funds</t>
+  </si>
+  <si>
+    <t>Ivy Variable Insurance Portfolios</t>
+  </si>
+  <si>
+    <t>JPMorgan Funds</t>
+  </si>
+  <si>
+    <t>Janus Henderson Funds</t>
+  </si>
+  <si>
+    <t>LEGG MASON</t>
+  </si>
+  <si>
+    <t>LORDABBETT</t>
+  </si>
+  <si>
+    <t>Litman Gregory</t>
+  </si>
+  <si>
+    <t>Longleaf Partners Funds</t>
+  </si>
+  <si>
+    <t>MARSICO INVESTMENT FUND</t>
+  </si>
+  <si>
+    <t>MERCERGLIN</t>
+  </si>
+  <si>
+    <t>MFS Funds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFS Funds </t>
+  </si>
+  <si>
+    <t>MORGAN STANLEY PATHWAY FUNDS</t>
+  </si>
+  <si>
+    <t>MainStay Group of Funds</t>
+  </si>
+  <si>
+    <t>Mainstay Group of Funds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetWest Funds </t>
+  </si>
+  <si>
+    <t>Morgan Stanley Funds</t>
+  </si>
+  <si>
+    <t>Mutual Fund Series Trust</t>
+  </si>
+  <si>
+    <t>Nationwide Mutual Funds</t>
+  </si>
+  <si>
+    <t>Natixis Loomis Sayles Funds</t>
+  </si>
+  <si>
+    <t>Northern Trust</t>
+  </si>
+  <si>
+    <t>Nuveen Funds</t>
+  </si>
+  <si>
+    <t>PACIFIC LIFE FUNDS</t>
+  </si>
+  <si>
+    <t>PAXWORLDFF</t>
+  </si>
+  <si>
+    <t>PENN Capital Funds Trust</t>
+  </si>
+  <si>
+    <t>PIMCOFUNDS</t>
+  </si>
+  <si>
+    <t>PRUDENTIAL</t>
+  </si>
+  <si>
+    <t>Pacific Life Funds</t>
+  </si>
+  <si>
+    <t>Parnassus Funds</t>
+  </si>
+  <si>
+    <t>Principal Exchange-Traded Funds</t>
+  </si>
+  <si>
+    <t>Procure ETF Trust II</t>
+  </si>
+  <si>
+    <t>Prudential</t>
+  </si>
+  <si>
+    <t>Putnam Family of Funds</t>
+  </si>
+  <si>
+    <t>ROYCEFUNDS</t>
+  </si>
+  <si>
+    <t>RUSSELLFDS</t>
+  </si>
+  <si>
+    <t>Renaissance Capital Greenwich Funds</t>
+  </si>
+  <si>
+    <t>RiverPark Funds</t>
+  </si>
+  <si>
+    <t>SA FUNDS INVESTMENT TRUST</t>
+  </si>
+  <si>
+    <t>SCHFLFSETF</t>
+  </si>
+  <si>
+    <t>SEI Funds</t>
+  </si>
+  <si>
+    <t>Salient Fund Complex</t>
+  </si>
+  <si>
+    <t>Segall Bryant &amp;amp; Hamill</t>
+  </si>
+  <si>
+    <t>Six Circles Funds</t>
+  </si>
+  <si>
+    <t>State Street Global Advisors - advised funds</t>
+  </si>
+  <si>
+    <t>Stone Harbor Investment Partner</t>
+  </si>
+  <si>
+    <t>THE ARBITRAGE FUNDS</t>
+  </si>
+  <si>
+    <t>THORNBURG</t>
+  </si>
+  <si>
+    <t>TIAA-CREF FUNDS COMPLEX</t>
+  </si>
+  <si>
+    <t>TIAA-CREF Funds Complex</t>
+  </si>
+  <si>
+    <t>TRANSAMERICA</t>
+  </si>
+  <si>
+    <t>TRUSTCOMPW</t>
+  </si>
+  <si>
+    <t>The Pioneer Funds</t>
+  </si>
+  <si>
+    <t>Third Avenue Funds</t>
+  </si>
+  <si>
+    <t>Thrivent Funds</t>
+  </si>
+  <si>
+    <t>Touchstone Funds</t>
+  </si>
+  <si>
+    <t>Transamerica</t>
+  </si>
+  <si>
+    <t>Trust for Credit Unions</t>
+  </si>
+  <si>
+    <t>UBSASSETMT</t>
+  </si>
+  <si>
+    <t>US Global Investors Funds</t>
+  </si>
+  <si>
+    <t>USAA Mutual Funds Trust</t>
+  </si>
+  <si>
+    <t>VANECKFUND</t>
+  </si>
+  <si>
+    <t>Victory Portfolios</t>
+  </si>
+  <si>
+    <t>Virtus ETFs</t>
+  </si>
+  <si>
+    <t>Virtus Funds</t>
+  </si>
+  <si>
+    <t>Wasatch Funds</t>
+  </si>
+  <si>
+    <t>Wells Fargo Funds</t>
+  </si>
+  <si>
+    <t>Westchester Capital Funds</t>
+  </si>
+  <si>
+    <t>Wilshire Mutual Funds</t>
+  </si>
+  <si>
+    <t>WisdomTree Trust</t>
+  </si>
+  <si>
+    <t>XTRACKERS</t>
+  </si>
+  <si>
+    <t>CAMBRIA INVESTMENT MANAGEMENT, LP</t>
+  </si>
+  <si>
+    <t>Crossmark Global Investments, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krane Funds Advisors, LLC                                                             </t>
+  </si>
+  <si>
+    <t>Perritt Funds, Inc.</t>
+  </si>
+  <si>
+    <t>The Vanguard Group, Inc.</t>
+  </si>
+  <si>
+    <t>Wilshire Mutual Funds, Inc.</t>
+  </si>
+  <si>
+    <t>Allianz</t>
+  </si>
+  <si>
+    <t>Alger</t>
+  </si>
+  <si>
+    <t>Cambria</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Kinetics Funds</t>
+  </si>
+  <si>
+    <t>Aberdeen Standard Investments</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>Alliance Bernstein</t>
+  </si>
+  <si>
+    <t>ALPS</t>
+  </si>
+  <si>
+    <t>AQR</t>
+  </si>
+  <si>
+    <t>Alpha Architect</t>
+  </si>
+  <si>
+    <t>AmericaFirst</t>
+  </si>
+  <si>
+    <t>BBH</t>
+  </si>
+  <si>
+    <t>Angel Oak</t>
+  </si>
+  <si>
+    <t>Ashmore Group</t>
+  </si>
+  <si>
+    <t>Bridge Builder</t>
+  </si>
+  <si>
+    <t>Cohen &amp; Steers</t>
+  </si>
+  <si>
+    <t>Community Capital</t>
+  </si>
+  <si>
+    <t>City National Rochdale</t>
+  </si>
+  <si>
+    <t>Direxion Shares ETF</t>
+  </si>
+  <si>
+    <t>DoubleLine</t>
+  </si>
+  <si>
+    <t>MetWest</t>
+  </si>
+  <si>
+    <t>Perritt</t>
+  </si>
+  <si>
+    <t>RiverPark</t>
+  </si>
+  <si>
+    <t>Salient</t>
+  </si>
+  <si>
+    <t>Wilshire</t>
+  </si>
+  <si>
+    <t>WisdomTree</t>
+  </si>
+  <si>
+    <t>GMO</t>
+  </si>
+  <si>
+    <t>Eaton Vance</t>
+  </si>
+  <si>
+    <t>JP Morgan</t>
+  </si>
+  <si>
+    <t>Janus Henderson</t>
+  </si>
+  <si>
+    <t>Legg Mason</t>
+  </si>
+  <si>
+    <t>Morgan Stanley</t>
+  </si>
+  <si>
+    <t>Nationwide Mutual</t>
+  </si>
+  <si>
+    <t>Nuveen</t>
+  </si>
+  <si>
+    <t>Pacific Life</t>
+  </si>
+  <si>
+    <t>PIMCO</t>
+  </si>
+  <si>
+    <t>State Street</t>
+  </si>
+  <si>
+    <t>Vanguard</t>
+  </si>
+  <si>
+    <t>UBS</t>
+  </si>
+  <si>
+    <t>USAA</t>
+  </si>
+  <si>
+    <t>First Trust Advisors</t>
+  </si>
+  <si>
+    <t>Lord Abbett</t>
+  </si>
+  <si>
+    <t>MainStay Funds</t>
+  </si>
+  <si>
+    <t>GAMCO</t>
+  </si>
+  <si>
+    <t>Global X</t>
+  </si>
+  <si>
+    <t>AssetMark</t>
+  </si>
+  <si>
+    <t>Innovator ETFs</t>
+  </si>
+  <si>
+    <t>Ivy Investments</t>
+  </si>
+  <si>
+    <t>Krane Funds</t>
+  </si>
+  <si>
+    <t>Longleaf Partners</t>
+  </si>
+  <si>
+    <t>Natixis</t>
+  </si>
+  <si>
+    <t>Parnassus</t>
+  </si>
+  <si>
+    <t>Putnam Investments</t>
+  </si>
+  <si>
+    <t>Royce Investment Partners</t>
+  </si>
+  <si>
+    <t>Renaissance Capital</t>
+  </si>
+  <si>
+    <t>Segall Bryant &amp; Hamill</t>
+  </si>
+  <si>
+    <t>Six Circles</t>
+  </si>
+  <si>
+    <t>Stone Harbor</t>
+  </si>
+  <si>
+    <t>The Arbitrage Funds</t>
+  </si>
+  <si>
+    <t>Thornburg Investment Management</t>
+  </si>
+  <si>
+    <t>TIAA</t>
+  </si>
+  <si>
+    <t>Third Avenue</t>
+  </si>
+  <si>
+    <t>Thrivent</t>
+  </si>
+  <si>
+    <t>Touchstone Investments</t>
+  </si>
+  <si>
+    <t>U.S. Global Investors</t>
+  </si>
+  <si>
+    <t>VanEck</t>
+  </si>
+  <si>
+    <t>Victory Capital</t>
+  </si>
+  <si>
+    <t>Virtus Investment Partners</t>
+  </si>
+  <si>
+    <t>Wasatch</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Westchester Capital</t>
+  </si>
+  <si>
+    <t>Xtrackers ETFs</t>
+  </si>
+  <si>
+    <t>EQ Advisors</t>
+  </si>
+  <si>
+    <t>Marisco</t>
+  </si>
+  <si>
+    <t>MSF</t>
+  </si>
+  <si>
+    <t>MFS</t>
+  </si>
+  <si>
+    <t>Pax World Funds</t>
+  </si>
+  <si>
+    <t>Penn Capital</t>
+  </si>
+  <si>
+    <t>Procure ETF</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>AMG</t>
+  </si>
+  <si>
+    <t>Glenmede</t>
+  </si>
+  <si>
+    <t>Mercer</t>
+  </si>
+  <si>
+    <t>Schwab</t>
+  </si>
+  <si>
+    <t>SEI</t>
+  </si>
+  <si>
+    <t>TCW</t>
+  </si>
+  <si>
+    <t>ETF Managers Group</t>
+  </si>
+  <si>
+    <t>Eventide</t>
+  </si>
+  <si>
+    <t>SA Funds</t>
+  </si>
+  <si>
+    <t>Pioneer</t>
+  </si>
+  <si>
+    <t>Investment Managers Series Trust</t>
   </si>
 </sst>
 </file>
@@ -654,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728DFE42-5040-4D37-A18F-76721B3D167B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -688,24 +1352,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,10 +1388,10 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -743,24 +1407,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,10 +1432,10 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +1474,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +1501,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -845,7 +1509,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -853,7 +1517,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -861,7 +1525,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -869,7 +1533,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -877,7 +1541,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -888,12 +1552,12 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -904,7 +1568,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -920,7 +1584,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +1616,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -984,7 +1648,7 @@
         <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,7 +1656,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1672,7 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1016,7 +1680,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1696,7 @@
         <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1712,7 @@
         <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,20 +1720,20 @@
         <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -1077,18 +1741,1285 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B050E7-7FFF-414C-8D97-6031501461B5}">
+  <dimension ref="A1:B156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="121.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>41</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>145</v>
+      </c>
+      <c r="B83" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>150</v>
+      </c>
+      <c r="B89" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>151</v>
+      </c>
+      <c r="B90" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>154</v>
+      </c>
+      <c r="B93" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>158</v>
+      </c>
+      <c r="B98" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>159</v>
+      </c>
+      <c r="B99" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>160</v>
+      </c>
+      <c r="B100" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>161</v>
+      </c>
+      <c r="B101" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
+      <c r="B103" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+      <c r="B104" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>165</v>
+      </c>
+      <c r="B105" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>167</v>
+      </c>
+      <c r="B109" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>47</v>
+      </c>
+      <c r="B111" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>169</v>
+      </c>
+      <c r="B112" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>172</v>
+      </c>
+      <c r="B115" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>173</v>
+      </c>
+      <c r="B116" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>174</v>
+      </c>
+      <c r="B117" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>175</v>
+      </c>
+      <c r="B118" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>48</v>
+      </c>
+      <c r="B120" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>177</v>
+      </c>
+      <c r="B121" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>178</v>
+      </c>
+      <c r="B122" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>50</v>
+      </c>
+      <c r="B123" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>179</v>
+      </c>
+      <c r="B124" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>180</v>
+      </c>
+      <c r="B125" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>181</v>
+      </c>
+      <c r="B126" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>182</v>
+      </c>
+      <c r="B127" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>183</v>
+      </c>
+      <c r="B128" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>184</v>
+      </c>
+      <c r="B129" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>185</v>
+      </c>
+      <c r="B130" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>186</v>
+      </c>
+      <c r="B131" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>51</v>
+      </c>
+      <c r="B132" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>187</v>
+      </c>
+      <c r="B133" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>188</v>
+      </c>
+      <c r="B134" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>211</v>
+      </c>
+      <c r="B135" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>189</v>
+      </c>
+      <c r="B136" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>190</v>
+      </c>
+      <c r="B137" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>191</v>
+      </c>
+      <c r="B138" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>192</v>
+      </c>
+      <c r="B139" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>193</v>
+      </c>
+      <c r="B140" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>194</v>
+      </c>
+      <c r="B141" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>195</v>
+      </c>
+      <c r="B142" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>196</v>
+      </c>
+      <c r="B143" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>52</v>
       </c>
-      <c r="B34" t="s">
-        <v>56</v>
+      <c r="B144" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>197</v>
+      </c>
+      <c r="B145" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>198</v>
+      </c>
+      <c r="B146" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>199</v>
+      </c>
+      <c r="B147" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>200</v>
+      </c>
+      <c r="B148" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>53</v>
+      </c>
+      <c r="B149" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>201</v>
+      </c>
+      <c r="B150" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>202</v>
+      </c>
+      <c r="B151" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>203</v>
+      </c>
+      <c r="B152" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>204</v>
+      </c>
+      <c r="B153" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>212</v>
+      </c>
+      <c r="B154" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>205</v>
+      </c>
+      <c r="B155" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>206</v>
+      </c>
+      <c r="B156" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summed up QoQ changes, moved graphing functions to graph_data, finished mapping out remaining fundManagers from fundManagers_raw created unicorn_summary file instead of generating each time for app_summary page, fixed reloading sending app to home page
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC8FDBB-486E-4772-9B0C-CBF516FC5F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F172925-7ECA-406B-A27D-D61B0CFEDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="2" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="allfund_map" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">allfund_map!$A$1:$B$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">allfund_map!$A$1:$B$240</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="448">
   <si>
     <t>T. Rowe Price</t>
   </si>
@@ -954,6 +954,435 @@
   </si>
   <si>
     <t>Investment Managers Series Trust</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>ADVISORS SERIES TRUST</t>
+  </si>
+  <si>
+    <t>ADVISORS' INNER CIRCLE FUND</t>
+  </si>
+  <si>
+    <t>AEGIS FUNDS</t>
+  </si>
+  <si>
+    <t>AFL CIO HOUSING INVESTMENT TRUST</t>
+  </si>
+  <si>
+    <t>ALPS Series Trust</t>
+  </si>
+  <si>
+    <t>AMERICAN PENSION INVESTORS TRUST</t>
+  </si>
+  <si>
+    <t>ARTISAN PARTNERS FUNDS INC</t>
+  </si>
+  <si>
+    <t>Adviser Managed Trust</t>
+  </si>
+  <si>
+    <t>Advisors' Inner Circle Fund II</t>
+  </si>
+  <si>
+    <t>Advisors' Inner Circle Fund III</t>
+  </si>
+  <si>
+    <t>Amplify ETF Trust</t>
+  </si>
+  <si>
+    <t>BRIDGEWAY FUNDS INC</t>
+  </si>
+  <si>
+    <t>BRUCE FUND INC</t>
+  </si>
+  <si>
+    <t>Barings Funds Trust</t>
+  </si>
+  <si>
+    <t>Brown Advisory Funds</t>
+  </si>
+  <si>
+    <t>CLEARWATER INVESTMENT TRUST</t>
+  </si>
+  <si>
+    <t>COLORADO BONDSHARES A TAX EXEMPT FUND</t>
+  </si>
+  <si>
+    <t>COMMONWEALTH INTERNATIONAL SERIES TRUST</t>
+  </si>
+  <si>
+    <t>Centre Funds</t>
+  </si>
+  <si>
+    <t>DRIEHAUS MUTUAL FUNDS</t>
+  </si>
+  <si>
+    <t>EMERGING MARKETS GROWTH FUND INC</t>
+  </si>
+  <si>
+    <t>ETF Series Solutions</t>
+  </si>
+  <si>
+    <t>Evermore Funds Trust</t>
+  </si>
+  <si>
+    <t>FIRSTHAND FUNDS</t>
+  </si>
+  <si>
+    <t>FlexShares Trust</t>
+  </si>
+  <si>
+    <t>Frost Family of Funds</t>
+  </si>
+  <si>
+    <t>GuideStone Funds</t>
+  </si>
+  <si>
+    <t>HARBOR FUNDS</t>
+  </si>
+  <si>
+    <t>HC CAPITAL TRUST</t>
+  </si>
+  <si>
+    <t>HOTCHKIS &amp; WILEY FUNDS /DE/</t>
+  </si>
+  <si>
+    <t>Jacob Funds Inc.</t>
+  </si>
+  <si>
+    <t>KIRR MARBACH PARTNERS FUNDS INC</t>
+  </si>
+  <si>
+    <t>LEUTHOLD FUNDS INC</t>
+  </si>
+  <si>
+    <t>LKCM Funds</t>
+  </si>
+  <si>
+    <t>LoCorr Investment Trust</t>
+  </si>
+  <si>
+    <t>M FUND INC</t>
+  </si>
+  <si>
+    <t>MANNING &amp; NAPIER FUND, INC.</t>
+  </si>
+  <si>
+    <t>MATTHEW 25 FUND</t>
+  </si>
+  <si>
+    <t>MATTHEWS INTERNATIONAL FUNDS</t>
+  </si>
+  <si>
+    <t>MERGER FUND</t>
+  </si>
+  <si>
+    <t>MERGER FUND VL</t>
+  </si>
+  <si>
+    <t>MERIDIAN FUND INC</t>
+  </si>
+  <si>
+    <t>MUTUAL OF AMERICA INVESTMENT CORP</t>
+  </si>
+  <si>
+    <t>Managed Portfolio Series</t>
+  </si>
+  <si>
+    <t>Meeder Funds</t>
+  </si>
+  <si>
+    <t>Morningstar Funds Trust</t>
+  </si>
+  <si>
+    <t>Mutual of America Variable Insurance Portfolios, Inc.</t>
+  </si>
+  <si>
+    <t>NEW ALTERNATIVES FUND</t>
+  </si>
+  <si>
+    <t>NORTHEAST INVESTORS TRUST</t>
+  </si>
+  <si>
+    <t>NORTHWESTERN MUTUAL SERIES FUND INC</t>
+  </si>
+  <si>
+    <t>North Square Investments Trust</t>
+  </si>
+  <si>
+    <t>Northern Lights Fund Trust</t>
+  </si>
+  <si>
+    <t>OCM MUTUAL FUND</t>
+  </si>
+  <si>
+    <t>OLD WESTBURY FUNDS INC</t>
+  </si>
+  <si>
+    <t>PPM Funds</t>
+  </si>
+  <si>
+    <t>PRIMECAP Odyssey Funds</t>
+  </si>
+  <si>
+    <t>PROFESSIONALLY MANAGED PORTFOLIOS</t>
+  </si>
+  <si>
+    <t>Pacer Funds Trust</t>
+  </si>
+  <si>
+    <t>QUAKER INVESTMENT TRUST</t>
+  </si>
+  <si>
+    <t>RBB FUND, INC.</t>
+  </si>
+  <si>
+    <t>RBC FUNDS TRUST</t>
+  </si>
+  <si>
+    <t>REYNOLDS FUNDS INC</t>
+  </si>
+  <si>
+    <t>RMB INVESTORS TRUST</t>
+  </si>
+  <si>
+    <t>RiverNorth Funds</t>
+  </si>
+  <si>
+    <t>SATURNA INVESTMENT TRUST</t>
+  </si>
+  <si>
+    <t>SPARROW FUNDS</t>
+  </si>
+  <si>
+    <t>SPIRIT OF AMERICA INVESTMENT FUND INC</t>
+  </si>
+  <si>
+    <t>Series Portfolios Trust</t>
+  </si>
+  <si>
+    <t>Symmetry Panoramic Trust</t>
+  </si>
+  <si>
+    <t>TANAKA FUNDS INC</t>
+  </si>
+  <si>
+    <t>TIFF INVESTMENT PROGRAM</t>
+  </si>
+  <si>
+    <t>TIMOTHY PLAN</t>
+  </si>
+  <si>
+    <t>TRUST FOR PROFESSIONAL MANAGERS</t>
+  </si>
+  <si>
+    <t>TWEEDY, BROWNE FUND INC.</t>
+  </si>
+  <si>
+    <t>Tidal ETF Trust</t>
+  </si>
+  <si>
+    <t>Trust for Advised Portfolios</t>
+  </si>
+  <si>
+    <t>Vericimetry Funds</t>
+  </si>
+  <si>
+    <t>WELLS FARGO MASTER TRUST</t>
+  </si>
+  <si>
+    <t>Bridgeway</t>
+  </si>
+  <si>
+    <t>Barings</t>
+  </si>
+  <si>
+    <t>Clearwater Investment Management</t>
+  </si>
+  <si>
+    <t>Evermore</t>
+  </si>
+  <si>
+    <t>Firsthand Funds</t>
+  </si>
+  <si>
+    <t>Frost Investment Advisors</t>
+  </si>
+  <si>
+    <t>GuideStone</t>
+  </si>
+  <si>
+    <t>Harbor Funds</t>
+  </si>
+  <si>
+    <t>Morningstar</t>
+  </si>
+  <si>
+    <t>Northwestern Mutual</t>
+  </si>
+  <si>
+    <t>North Square</t>
+  </si>
+  <si>
+    <t>Nothern Light</t>
+  </si>
+  <si>
+    <t>Pacer</t>
+  </si>
+  <si>
+    <t>RiverNorth</t>
+  </si>
+  <si>
+    <t>Saturna</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
+  </si>
+  <si>
+    <t>Tanaka</t>
+  </si>
+  <si>
+    <t>Tidal ETF</t>
+  </si>
+  <si>
+    <t>Vericimetry</t>
+  </si>
+  <si>
+    <t>Artisan Partners</t>
+  </si>
+  <si>
+    <t>Aegis</t>
+  </si>
+  <si>
+    <t>Bruce Fund</t>
+  </si>
+  <si>
+    <t>Brown Advisory</t>
+  </si>
+  <si>
+    <t>Driehaus</t>
+  </si>
+  <si>
+    <t>LoCorr</t>
+  </si>
+  <si>
+    <t>Hotchkis &amp; Wiley</t>
+  </si>
+  <si>
+    <t>Jacob Funds</t>
+  </si>
+  <si>
+    <t>Matthews</t>
+  </si>
+  <si>
+    <t>Matthew 25</t>
+  </si>
+  <si>
+    <t>Meridian</t>
+  </si>
+  <si>
+    <t>Mutual of America</t>
+  </si>
+  <si>
+    <t>RBC</t>
+  </si>
+  <si>
+    <t>Sparrow</t>
+  </si>
+  <si>
+    <t>Spirit of America</t>
+  </si>
+  <si>
+    <t>Symmetry Partners</t>
+  </si>
+  <si>
+    <t>TIFF</t>
+  </si>
+  <si>
+    <t>Tweedy, Browne</t>
+  </si>
+  <si>
+    <t>Manning &amp; Napier</t>
+  </si>
+  <si>
+    <t>Leuthold</t>
+  </si>
+  <si>
+    <t>LKCM</t>
+  </si>
+  <si>
+    <t>Kirr, Marbach Partners</t>
+  </si>
+  <si>
+    <t>HC Capital Trust</t>
+  </si>
+  <si>
+    <t>FlexShares</t>
+  </si>
+  <si>
+    <t>Northeast Investors Trust</t>
+  </si>
+  <si>
+    <t>OCM Funds</t>
+  </si>
+  <si>
+    <t>Old Westbury Funds</t>
+  </si>
+  <si>
+    <t>PRIMECAP</t>
+  </si>
+  <si>
+    <t>Quaker Investment Trust</t>
+  </si>
+  <si>
+    <t>Amplify ETF</t>
+  </si>
+  <si>
+    <t>Merger Fund</t>
+  </si>
+  <si>
+    <t>RBB Fund</t>
+  </si>
+  <si>
+    <t>RMB Funds</t>
+  </si>
+  <si>
+    <t>Timothy Plan</t>
+  </si>
+  <si>
+    <t>New Alternatives Fund</t>
+  </si>
+  <si>
+    <t>Advisors Series Trust</t>
+  </si>
+  <si>
+    <t>AFL-CIO</t>
+  </si>
+  <si>
+    <t>American Pension Investors Trust</t>
+  </si>
+  <si>
+    <t>Colorado BondShares</t>
+  </si>
+  <si>
+    <t>Commonwealth Funds</t>
+  </si>
+  <si>
+    <t>Emerging Markets Growth Fund</t>
+  </si>
+  <si>
+    <t>Osterweis</t>
+  </si>
+  <si>
+    <t>Weiss</t>
+  </si>
+  <si>
+    <t>Trust for Professional Managers</t>
+  </si>
+  <si>
+    <t>Advisors' Inner Circle</t>
   </si>
 </sst>
 </file>
@@ -998,9 +1427,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1762,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B050E7-7FFF-414C-8D97-6031501461B5}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,7 +2221,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -3020,6 +3450,686 @@
       </c>
       <c r="B156" t="s">
         <v>285</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>306</v>
+      </c>
+      <c r="B157" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>307</v>
+      </c>
+      <c r="B158" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>308</v>
+      </c>
+      <c r="B159" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>309</v>
+      </c>
+      <c r="B160" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>310</v>
+      </c>
+      <c r="B161" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>311</v>
+      </c>
+      <c r="B162" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>312</v>
+      </c>
+      <c r="B163" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>313</v>
+      </c>
+      <c r="B164" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>314</v>
+      </c>
+      <c r="B165" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>315</v>
+      </c>
+      <c r="B166" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>316</v>
+      </c>
+      <c r="B167" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>317</v>
+      </c>
+      <c r="B168" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>318</v>
+      </c>
+      <c r="B169" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>319</v>
+      </c>
+      <c r="B170" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>69</v>
+      </c>
+      <c r="B171" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>70</v>
+      </c>
+      <c r="B172" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>71</v>
+      </c>
+      <c r="B173" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>320</v>
+      </c>
+      <c r="B174" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>321</v>
+      </c>
+      <c r="B175" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>322</v>
+      </c>
+      <c r="B176" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>323</v>
+      </c>
+      <c r="B177" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>324</v>
+      </c>
+      <c r="B178" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>72</v>
+      </c>
+      <c r="B179" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>325</v>
+      </c>
+      <c r="B180" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>326</v>
+      </c>
+      <c r="B181" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>327</v>
+      </c>
+      <c r="B182" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>328</v>
+      </c>
+      <c r="B183" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>329</v>
+      </c>
+      <c r="B184" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>330</v>
+      </c>
+      <c r="B185" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>331</v>
+      </c>
+      <c r="B186" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>35</v>
+      </c>
+      <c r="B187" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>332</v>
+      </c>
+      <c r="B188" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>333</v>
+      </c>
+      <c r="B189" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>334</v>
+      </c>
+      <c r="B190" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>335</v>
+      </c>
+      <c r="B191" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>336</v>
+      </c>
+      <c r="B192" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>337</v>
+      </c>
+      <c r="B193" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>338</v>
+      </c>
+      <c r="B194" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>339</v>
+      </c>
+      <c r="B195" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>340</v>
+      </c>
+      <c r="B196" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>341</v>
+      </c>
+      <c r="B197" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>342</v>
+      </c>
+      <c r="B198" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>343</v>
+      </c>
+      <c r="B199" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>344</v>
+      </c>
+      <c r="B200" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>345</v>
+      </c>
+      <c r="B201" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>346</v>
+      </c>
+      <c r="B202" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>347</v>
+      </c>
+      <c r="B203" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>348</v>
+      </c>
+      <c r="B204" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>349</v>
+      </c>
+      <c r="B205" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>350</v>
+      </c>
+      <c r="B206" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>351</v>
+      </c>
+      <c r="B207" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>352</v>
+      </c>
+      <c r="B208" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>353</v>
+      </c>
+      <c r="B209" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>354</v>
+      </c>
+      <c r="B210" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>355</v>
+      </c>
+      <c r="B211" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>356</v>
+      </c>
+      <c r="B212" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>357</v>
+      </c>
+      <c r="B213" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>358</v>
+      </c>
+      <c r="B214" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>359</v>
+      </c>
+      <c r="B215" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>45</v>
+      </c>
+      <c r="B216" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>360</v>
+      </c>
+      <c r="B217" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>361</v>
+      </c>
+      <c r="B218" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>362</v>
+      </c>
+      <c r="B219" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>363</v>
+      </c>
+      <c r="B220" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>364</v>
+      </c>
+      <c r="B221" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>365</v>
+      </c>
+      <c r="B222" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>366</v>
+      </c>
+      <c r="B223" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>367</v>
+      </c>
+      <c r="B224" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>368</v>
+      </c>
+      <c r="B225" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>369</v>
+      </c>
+      <c r="B226" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>370</v>
+      </c>
+      <c r="B227" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>371</v>
+      </c>
+      <c r="B228" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>372</v>
+      </c>
+      <c r="B229" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>373</v>
+      </c>
+      <c r="B230" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>374</v>
+      </c>
+      <c r="B231" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>375</v>
+      </c>
+      <c r="B232" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>376</v>
+      </c>
+      <c r="B233" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>377</v>
+      </c>
+      <c r="B234" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>378</v>
+      </c>
+      <c r="B235" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>379</v>
+      </c>
+      <c r="B236" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>380</v>
+      </c>
+      <c r="B237" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>381</v>
+      </c>
+      <c r="B238" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>382</v>
+      </c>
+      <c r="B239" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>383</v>
+      </c>
+      <c r="B240" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>305</v>
+      </c>
+      <c r="B241" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor tweak to home page, small edit to fundManager file
</commit_message>
<xml_diff>
--- a/data/master_funds.xlsx
+++ b/data/master_funds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miket\OneDrive\Desktop\ML\Projects\fundvaluations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F172925-7ECA-406B-A27D-D61B0CFEDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BDA009-B9EA-4633-A81A-250BEE436276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="2" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
+    <workbookView xWindow="30" yWindow="780" windowWidth="28770" windowHeight="14820" activeTab="2" xr2:uid="{0DB00A2D-3235-4721-B852-C489DA525686}"/>
   </bookViews>
   <sheets>
     <sheet name="fund_details" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="449">
   <si>
     <t>T. Rowe Price</t>
   </si>
@@ -1383,6 +1383,9 @@
   </si>
   <si>
     <t>Advisors' Inner Circle</t>
+  </si>
+  <si>
+    <t>SunAmerica</t>
   </si>
 </sst>
 </file>
@@ -2194,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B050E7-7FFF-414C-8D97-6031501461B5}">
   <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,7 +3164,7 @@
         <v>48</v>
       </c>
       <c r="B120" t="s">
-        <v>58</v>
+        <v>448</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>